<commit_message>
Added some comments to the activities
</commit_message>
<xml_diff>
--- a/Database/Employee_payroll_table_07_07_2020.xlsx
+++ b/Database/Employee_payroll_table_07_07_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\premal\Google Drive\QAC projects\HR automation\automation\HR-Payroll-automation\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153D0442-B90A-462B-9BF5-5E10C4424A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97693CAA-D79F-4E54-AB31-E604FB18F17B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20760" yWindow="2835" windowWidth="3240" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="128">
   <si>
     <t>Ryan</t>
   </si>
@@ -417,42 +417,6 @@
   </si>
   <si>
     <t xml:space="preserve"> £    18.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,920.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £     800.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,760.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,600.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,120.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £     640.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,040.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,680.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £     960.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  2,000.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,280.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> £  1,440.00 </t>
   </si>
 </sst>
 </file>
@@ -488,8 +452,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,9 +772,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -847,7 +818,7 @@
       <c r="L1" t="s">
         <v>109</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
@@ -888,8 +859,8 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>128</v>
+      <c r="M2" s="2">
+        <v>1920</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -929,7 +900,7 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <f>H3*I3</f>
         <v>110</v>
       </c>
@@ -971,8 +942,8 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" t="s">
-        <v>130</v>
+      <c r="M4" s="2">
+        <v>1760</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1012,8 +983,8 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
-        <v>131</v>
+      <c r="M5" s="2">
+        <v>1600</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1053,8 +1024,8 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
-        <v>130</v>
+      <c r="M6" s="2">
+        <v>1760</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1094,8 +1065,8 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7" t="s">
-        <v>132</v>
+      <c r="M7" s="2">
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1135,8 +1106,8 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" t="s">
-        <v>129</v>
+      <c r="M8" s="1">
+        <v>800</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1176,8 +1147,8 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" t="s">
-        <v>133</v>
+      <c r="M9" s="1">
+        <v>640</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1217,8 +1188,8 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>134</v>
+      <c r="M10" s="2">
+        <v>1040</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1258,8 +1229,8 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>135</v>
+      <c r="M11" s="2">
+        <v>1680</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1299,8 +1270,8 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" t="s">
-        <v>134</v>
+      <c r="M12" s="2">
+        <v>1040</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1340,8 +1311,8 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" t="s">
-        <v>128</v>
+      <c r="M13" s="2">
+        <v>1920</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1381,8 +1352,8 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" t="s">
-        <v>136</v>
+      <c r="M14" s="1">
+        <v>960</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1422,8 +1393,8 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" t="s">
-        <v>137</v>
+      <c r="M15" s="2">
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1463,8 +1434,8 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" t="s">
-        <v>138</v>
+      <c r="M16" s="2">
+        <v>1280</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1504,8 +1475,8 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
-        <v>139</v>
+      <c r="M17" s="2">
+        <v>1440</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1545,8 +1516,8 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" t="s">
-        <v>131</v>
+      <c r="M18" s="2">
+        <v>1600</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1586,8 +1557,8 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" t="s">
-        <v>138</v>
+      <c r="M19" s="2">
+        <v>1280</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1627,8 +1598,8 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" t="s">
-        <v>129</v>
+      <c r="M20" s="1">
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1668,11 +1639,12 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" t="s">
-        <v>139</v>
+      <c r="M21" s="2">
+        <v>1440</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>